<commit_message>
everything is working fine
</commit_message>
<xml_diff>
--- a/customSim/LES/systemDefinition/Order.xlsx
+++ b/customSim/LES/systemDefinition/Order.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:G1"/>
+  <dimension ref="B1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,6 @@
           <t>product</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>kwargs</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added upstream and downstream back to the sheet from system definition
</commit_message>
<xml_diff>
--- a/customSim/LES/systemDefinition/Order.xlsx
+++ b/customSim/LES/systemDefinition/Order.xlsx
@@ -2,27 +2,40 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="1710" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Order" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -37,12 +50,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,14 +83,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -425,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:F1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,29 +468,253 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>env</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>order_date</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>customer_name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>order_id</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>product</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>45317</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>name_1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>ord_1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>45320</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>name_2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ord_2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>45328</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>name_3</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>ord_3</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>45332</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>name_1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ord_4</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>45341</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>name_5</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ord_5</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>45350</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>name_6</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>ord_6</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>45357</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>name_1</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ord_7</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>env</t>
+        </is>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>45359</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>name_8</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>ord_8</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>{}</t>
         </is>
       </c>
     </row>

</xml_diff>